<commit_message>
* Nowe wyniki dla uint i usuniecie nieuzywanych kerneli
</commit_message>
<xml_diff>
--- a/morph-cl/Porownanie.xlsx
+++ b/morph-cl/Porownanie.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Rozmiar</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>"GFLOPS"</t>
+  </si>
+  <si>
+    <t>erode_c4_pragma</t>
+  </si>
+  <si>
+    <t>_c4_unroll jest w zasadzie identyczne co _c4</t>
   </si>
 </sst>
 </file>
@@ -1091,23 +1097,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="47753472"/>
-        <c:axId val="48168960"/>
+        <c:axId val="87091072"/>
+        <c:axId val="87092608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="47753472"/>
+        <c:axId val="87091072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48168960"/>
+        <c:crossAx val="87092608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48168960"/>
+        <c:axId val="87092608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1115,14 +1121,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47753472"/>
+        <c:crossAx val="87091072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3017,23 +3022,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="48895104"/>
-        <c:axId val="48896640"/>
+        <c:axId val="90051328"/>
+        <c:axId val="90052864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48895104"/>
+        <c:axId val="90051328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48896640"/>
+        <c:crossAx val="90052864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="48896640"/>
+        <c:axId val="90052864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
@@ -3042,14 +3047,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="48895104"/>
+        <c:crossAx val="90051328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3417,17 +3421,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AB41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="3" max="3" width="9.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="12.625" customWidth="1"/>
     <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.75" bestFit="1" customWidth="1"/>
@@ -3474,7 +3478,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>5</v>
@@ -6962,6 +6966,11 @@
       <c r="U40">
         <f>S40/T40</f>
         <v>200.39357303186023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
+      <c r="B41" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>